<commit_message>
Implemented UOM column to Spreadsheet export. Updated unittests.
</commit_message>
<xml_diff>
--- a/src/Tests/pickles/change_worksheet2_output.xlsx
+++ b/src/Tests/pickles/change_worksheet2_output.xlsx
@@ -506,21 +506,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N21"/>
+  <dimension ref="B2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:15">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
-      <c r="E2" s="2">
-        <v>0</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="2">
         <v>0</v>
       </c>
@@ -548,16 +546,17 @@
       <c r="N2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:14">
+      <c r="O2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="2">
-        <v>0</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="2">
         <v>0</v>
       </c>
@@ -585,16 +584,17 @@
       <c r="N3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="O3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="2">
         <v>0</v>
       </c>
@@ -622,16 +622,17 @@
       <c r="N4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="O4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="2">
         <v>0</v>
       </c>
@@ -659,16 +660,17 @@
       <c r="N5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
+      <c r="O5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
-      <c r="E6" s="2">
-        <v>0</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="2">
         <v>0</v>
       </c>
@@ -696,16 +698,17 @@
       <c r="N6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:14">
+      <c r="O6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="2">
-        <v>0</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="2">
         <v>0</v>
       </c>
@@ -733,16 +736,17 @@
       <c r="N7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
+      <c r="O7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="2">
-        <v>0</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="2">
         <v>0</v>
       </c>
@@ -770,16 +774,17 @@
       <c r="N8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="O8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="2">
-        <v>0</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="2">
         <v>0</v>
       </c>
@@ -807,16 +812,17 @@
       <c r="N9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
+      <c r="O9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="2">
-        <v>0</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="2">
         <v>0</v>
       </c>
@@ -844,16 +850,17 @@
       <c r="N10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="O10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="2">
-        <v>0</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="2">
         <v>0</v>
       </c>
@@ -881,16 +888,17 @@
       <c r="N11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="O11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="2">
-        <v>0</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="2">
         <v>0</v>
       </c>
@@ -918,16 +926,17 @@
       <c r="N12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
+      <c r="O12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="2">
-        <v>0</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="2">
         <v>0</v>
       </c>
@@ -955,16 +964,17 @@
       <c r="N13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:14">
+      <c r="O13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="2">
-        <v>0</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="2">
         <v>0</v>
       </c>
@@ -992,16 +1002,17 @@
       <c r="N14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:14">
+      <c r="O14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="2">
-        <v>0</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="2">
         <v>0</v>
       </c>
@@ -1029,16 +1040,17 @@
       <c r="N15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:14">
+      <c r="O15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="2">
-        <v>0</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="2">
         <v>0</v>
       </c>
@@ -1066,16 +1078,17 @@
       <c r="N17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:14">
+      <c r="O17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="2">
-        <v>0</v>
-      </c>
+      <c r="E18" s="1"/>
       <c r="F18" s="2">
         <v>0</v>
       </c>
@@ -1103,16 +1116,17 @@
       <c r="N18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:14">
+      <c r="O18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="2">
-        <v>0</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="2">
         <v>0</v>
       </c>
@@ -1140,16 +1154,17 @@
       <c r="N19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:14">
+      <c r="O19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="2">
-        <v>0</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="2">
         <v>0</v>
       </c>
@@ -1177,16 +1192,17 @@
       <c r="N20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:14">
+      <c r="O20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="2">
-        <v>0</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="2">
         <v>0</v>
       </c>
@@ -1212,6 +1228,9 @@
         <v>0</v>
       </c>
       <c r="N21" s="2">
+        <v>0</v>
+      </c>
+      <c r="O21" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1222,22 +1241,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N57"/>
+  <dimension ref="B2:O57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:15">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="3">
-        <f>E30</f>
-        <v>0</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="3">
         <f>F30</f>
         <v>0</v>
@@ -1274,17 +1290,18 @@
         <f>N30</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:14">
+      <c r="O2" s="3">
+        <f>O30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="4">
-        <f>Inputs!E$2</f>
-        <v>0</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="4">
         <f>Inputs!F$2</f>
         <v>0</v>
@@ -1321,17 +1338,18 @@
         <f>Inputs!N$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="O3" s="4">
+        <f>Inputs!O$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="3">
-        <f>E2+E3</f>
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="3">
         <f>F2+F3</f>
         <v>0</v>
@@ -1368,17 +1386,18 @@
         <f>N2+N3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="O4" s="3">
+        <f>O2+O3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="4">
-        <f>Inputs!E$3</f>
-        <v>0</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="4">
         <f>Inputs!F$3</f>
         <v>0</v>
@@ -1415,17 +1434,18 @@
         <f>Inputs!N$3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:14">
+      <c r="O5" s="4">
+        <f>Inputs!O$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:15">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="3">
-        <f>E5+E4</f>
-        <v>0</v>
-      </c>
+      <c r="E6" s="1"/>
       <c r="F6" s="3">
         <f>F5+F4</f>
         <v>0</v>
@@ -1462,17 +1482,18 @@
         <f>N5+N4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
+      <c r="O6" s="3">
+        <f>O5+O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4">
-        <f>Inputs!E$4</f>
-        <v>0</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="4">
         <f>Inputs!F$4</f>
         <v>0</v>
@@ -1509,17 +1530,18 @@
         <f>Inputs!N$4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="O8" s="4">
+        <f>Inputs!O$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="3">
-        <f>E32</f>
-        <v>0</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="3">
         <f>F32</f>
         <v>0</v>
@@ -1556,17 +1578,18 @@
         <f>N32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:14">
+      <c r="O9" s="3">
+        <f>O32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="1"/>
-      <c r="E10" s="3">
-        <f>E8+E9</f>
-        <v>0</v>
-      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="3">
         <f>F8+F9</f>
         <v>0</v>
@@ -1603,17 +1626,18 @@
         <f>N8+N9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="O10" s="3">
+        <f>O8+O9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="4">
-        <f>Inputs!E$5</f>
-        <v>0</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="4">
         <f>Inputs!F$5</f>
         <v>0</v>
@@ -1650,17 +1674,18 @@
         <f>Inputs!N$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="O11" s="4">
+        <f>Inputs!O$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="3">
-        <f>E11+E10</f>
-        <v>0</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="3">
         <f>F11+F10</f>
         <v>0</v>
@@ -1697,17 +1722,18 @@
         <f>N11+N10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:14">
+      <c r="O12" s="3">
+        <f>O11+O10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="4">
-        <f>Inputs!E$6</f>
-        <v>0</v>
-      </c>
+      <c r="E14" s="1"/>
       <c r="F14" s="4">
         <f>Inputs!F$6</f>
         <v>0</v>
@@ -1744,17 +1770,18 @@
         <f>Inputs!N$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:14">
+      <c r="O14" s="4">
+        <f>Inputs!O$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
-      <c r="E15" s="3">
-        <f>Model!E5</f>
-        <v>0</v>
-      </c>
+      <c r="E15" s="1"/>
       <c r="F15" s="3">
         <f>Model!F5</f>
         <v>0</v>
@@ -1791,17 +1818,18 @@
         <f>Model!N5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:14">
+      <c r="O15" s="3">
+        <f>Model!O5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1"/>
-      <c r="E16" s="4">
-        <f>Inputs!E$7</f>
-        <v>0</v>
-      </c>
+      <c r="E16" s="1"/>
       <c r="F16" s="4">
         <f>Inputs!F$7</f>
         <v>0</v>
@@ -1838,17 +1866,18 @@
         <f>Inputs!N$7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:14">
+      <c r="O16" s="4">
+        <f>Inputs!O$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15">
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="1"/>
-      <c r="E17" s="3">
-        <f>E16+E15+E14</f>
-        <v>0</v>
-      </c>
+      <c r="E17" s="1"/>
       <c r="F17" s="3">
         <f>F16+F15+F14</f>
         <v>0</v>
@@ -1885,17 +1914,18 @@
         <f>N16+N15+N14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:14">
+      <c r="O17" s="3">
+        <f>O16+O15+O14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15">
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="1"/>
-      <c r="E19" s="3">
-        <f>E17</f>
-        <v>0</v>
-      </c>
+      <c r="E19" s="1"/>
       <c r="F19" s="3">
         <f>F17</f>
         <v>0</v>
@@ -1932,17 +1962,18 @@
         <f>N17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:14">
+      <c r="O19" s="3">
+        <f>O17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="3">
-        <f>E8</f>
-        <v>0</v>
-      </c>
+      <c r="E20" s="1"/>
       <c r="F20" s="3">
         <f>F8</f>
         <v>0</v>
@@ -1979,17 +2010,18 @@
         <f>N8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:14">
+      <c r="O20" s="3">
+        <f>O8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15">
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="1"/>
-      <c r="E21" s="3">
-        <f>E11</f>
-        <v>0</v>
-      </c>
+      <c r="E21" s="1"/>
       <c r="F21" s="3">
         <f>F11</f>
         <v>0</v>
@@ -2026,17 +2058,18 @@
         <f>N11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:14">
+      <c r="O21" s="3">
+        <f>O11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15">
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="1"/>
-      <c r="E23" s="3">
-        <f>E3</f>
-        <v>0</v>
-      </c>
+      <c r="E23" s="1"/>
       <c r="F23" s="3">
         <f>F3</f>
         <v>0</v>
@@ -2073,17 +2106,18 @@
         <f>N3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:14">
+      <c r="O23" s="3">
+        <f>O3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15">
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1"/>
-      <c r="E24" s="3">
-        <f>E5</f>
-        <v>0</v>
-      </c>
+      <c r="E24" s="1"/>
       <c r="F24" s="3">
         <f>F5</f>
         <v>0</v>
@@ -2120,17 +2154,18 @@
         <f>N5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:14">
+      <c r="O24" s="3">
+        <f>O5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="1"/>
-      <c r="E25" s="3">
-        <f>E23+E24</f>
-        <v>0</v>
-      </c>
+      <c r="E25" s="1"/>
       <c r="F25" s="3">
         <f>F23+F24</f>
         <v>0</v>
@@ -2167,17 +2202,18 @@
         <f>N23+N24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:14">
+      <c r="O25" s="3">
+        <f>O23+O24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15">
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="1"/>
-      <c r="E27" s="3">
-        <f>E19+E20+E21-E25</f>
-        <v>0</v>
-      </c>
+      <c r="E27" s="1"/>
       <c r="F27" s="3">
         <f>F19+F20+F21-F25</f>
         <v>0</v>
@@ -2214,17 +2250,18 @@
         <f>N19+N20+N21-N25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:14">
+      <c r="O27" s="3">
+        <f>O19+O20+O21-O25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="3">
-        <f>max(0, E27)</f>
-        <v>0</v>
-      </c>
+      <c r="E29" s="1"/>
       <c r="F29" s="3">
         <f>max(0, F27)</f>
         <v>0</v>
@@ -2261,17 +2298,18 @@
         <f>max(0, N27)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:14">
+      <c r="O29" s="3">
+        <f>max(0, O27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="1"/>
-      <c r="E30" s="3">
-        <f>E29</f>
-        <v>0</v>
-      </c>
+      <c r="E30" s="1"/>
       <c r="F30" s="3">
         <f>F29</f>
         <v>0</v>
@@ -2308,17 +2346,18 @@
         <f>N29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:14">
+      <c r="O30" s="3">
+        <f>O29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="1"/>
-      <c r="E31" s="3">
-        <f>min(E27, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="E31" s="1"/>
       <c r="F31" s="3">
         <f>min(F27, 0)</f>
         <v>0</v>
@@ -2355,17 +2394,18 @@
         <f>min(N27, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:14">
+      <c r="O31" s="3">
+        <f>min(O27, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15">
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="3">
-        <f>-1*E31</f>
-        <v>0</v>
-      </c>
+      <c r="E32" s="1"/>
       <c r="F32" s="3">
         <f>-1*F31</f>
         <v>0</v>
@@ -2402,17 +2442,18 @@
         <f>-1*N31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:14">
+      <c r="O32" s="3">
+        <f>-1*O31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="1"/>
-      <c r="E34" s="3">
-        <f>E6</f>
-        <v>0</v>
-      </c>
+      <c r="E34" s="1"/>
       <c r="F34" s="3">
         <f>F6</f>
         <v>0</v>
@@ -2449,17 +2490,18 @@
         <f>N6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:14">
+      <c r="O34" s="3">
+        <f>O6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="3">
-        <f>E12</f>
-        <v>0</v>
-      </c>
+      <c r="E35" s="1"/>
       <c r="F35" s="3">
         <f>F12</f>
         <v>0</v>
@@ -2496,17 +2538,18 @@
         <f>N12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:14">
+      <c r="O35" s="3">
+        <f>O12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15">
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="1"/>
-      <c r="E36" s="3">
-        <f>E17</f>
-        <v>0</v>
-      </c>
+      <c r="E36" s="1"/>
       <c r="F36" s="3">
         <f>F17</f>
         <v>0</v>
@@ -2543,17 +2586,18 @@
         <f>N17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:14">
+      <c r="O36" s="3">
+        <f>O17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15">
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1"/>
-      <c r="E37" s="3">
-        <f>E34-(E35+E36)</f>
-        <v>0</v>
-      </c>
+      <c r="E37" s="1"/>
       <c r="F37" s="3">
         <f>F34-(F35+F36)</f>
         <v>0</v>
@@ -2590,17 +2634,18 @@
         <f>N34-(N35+N36)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:14">
+      <c r="O37" s="3">
+        <f>O34-(O35+O36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="1"/>
-      <c r="E39" s="3">
-        <f>'Core Accounts'!E2</f>
-        <v>0</v>
-      </c>
+      <c r="E39" s="1"/>
       <c r="F39" s="3">
         <f>'Core Accounts'!F2</f>
         <v>0</v>
@@ -2637,17 +2682,18 @@
         <f>'Core Accounts'!N2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:14">
+      <c r="O39" s="3">
+        <f>'Core Accounts'!O2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15">
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="1"/>
-      <c r="E40" s="3">
-        <f>'Core Accounts'!E4</f>
-        <v>0</v>
-      </c>
+      <c r="E40" s="1"/>
       <c r="F40" s="3">
         <f>'Core Accounts'!F4</f>
         <v>0</v>
@@ -2684,17 +2730,18 @@
         <f>'Core Accounts'!N4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:14">
+      <c r="O40" s="3">
+        <f>'Core Accounts'!O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15">
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D41" s="1"/>
-      <c r="E41" s="3">
-        <f>E39-E40</f>
-        <v>0</v>
-      </c>
+      <c r="E41" s="1"/>
       <c r="F41" s="3">
         <f>F39-F40</f>
         <v>0</v>
@@ -2731,17 +2778,18 @@
         <f>N39-N40</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:14">
+      <c r="O41" s="3">
+        <f>O39-O40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15">
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="1"/>
-      <c r="E43" s="4">
-        <f>Inputs!E$8</f>
-        <v>0</v>
-      </c>
+      <c r="E43" s="1"/>
       <c r="F43" s="4">
         <f>Inputs!F$8</f>
         <v>0</v>
@@ -2778,17 +2826,18 @@
         <f>Inputs!N$8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:14">
+      <c r="O43" s="4">
+        <f>Inputs!O$8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15">
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="1"/>
-      <c r="E44" s="4">
-        <f>Inputs!E$9</f>
-        <v>0</v>
-      </c>
+      <c r="E44" s="1"/>
       <c r="F44" s="4">
         <f>Inputs!F$9</f>
         <v>0</v>
@@ -2825,17 +2874,18 @@
         <f>Inputs!N$9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:14">
+      <c r="O44" s="4">
+        <f>Inputs!O$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15">
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1"/>
-      <c r="E45" s="4">
-        <f>Inputs!E$10</f>
-        <v>0</v>
-      </c>
+      <c r="E45" s="1"/>
       <c r="F45" s="4">
         <f>Inputs!F$10</f>
         <v>0</v>
@@ -2872,17 +2922,18 @@
         <f>Inputs!N$10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:14">
+      <c r="O45" s="4">
+        <f>Inputs!O$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15">
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="1"/>
-      <c r="E46" s="3">
-        <f>E41-(E43+E44)+E45</f>
-        <v>0</v>
-      </c>
+      <c r="E46" s="1"/>
       <c r="F46" s="3">
         <f>F41-(F43+F44)+F45</f>
         <v>0</v>
@@ -2919,17 +2970,18 @@
         <f>N41-(N43+N44)+N45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:14">
+      <c r="O46" s="3">
+        <f>O41-(O43+O44)+O45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:15">
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1"/>
-      <c r="E48" s="4">
-        <f>Inputs!E$11</f>
-        <v>0</v>
-      </c>
+      <c r="E48" s="1"/>
       <c r="F48" s="4">
         <f>Inputs!F$11</f>
         <v>0</v>
@@ -2966,17 +3018,18 @@
         <f>Inputs!N$11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:14">
+      <c r="O48" s="4">
+        <f>Inputs!O$11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:15">
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="1"/>
-      <c r="E49" s="4">
-        <f>Inputs!E$12</f>
-        <v>0</v>
-      </c>
+      <c r="E49" s="1"/>
       <c r="F49" s="4">
         <f>Inputs!F$12</f>
         <v>0</v>
@@ -3013,17 +3066,18 @@
         <f>Inputs!N$12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:14">
+      <c r="O49" s="4">
+        <f>Inputs!O$12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:15">
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D50" s="1"/>
-      <c r="E50" s="3">
-        <f>E46-(E48+E49)</f>
-        <v>0</v>
-      </c>
+      <c r="E50" s="1"/>
       <c r="F50" s="3">
         <f>F46-(F48+F49)</f>
         <v>0</v>
@@ -3060,17 +3114,18 @@
         <f>N46-(N48+N49)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:14">
+      <c r="O50" s="3">
+        <f>O46-(O48+O49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:15">
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="1"/>
-      <c r="E52" s="4">
-        <f>Inputs!E$13</f>
-        <v>0</v>
-      </c>
+      <c r="E52" s="1"/>
       <c r="F52" s="4">
         <f>Inputs!F$13</f>
         <v>0</v>
@@ -3107,17 +3162,18 @@
         <f>Inputs!N$13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:14">
+      <c r="O52" s="4">
+        <f>Inputs!O$13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:15">
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="4">
-        <f>Inputs!E$14</f>
-        <v>0</v>
-      </c>
+      <c r="E53" s="1"/>
       <c r="F53" s="4">
         <f>Inputs!F$14</f>
         <v>0</v>
@@ -3154,17 +3210,18 @@
         <f>Inputs!N$14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:14">
+      <c r="O53" s="4">
+        <f>Inputs!O$14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:15">
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D54" s="1"/>
-      <c r="E54" s="3">
-        <f>E50-E52+E53</f>
-        <v>0</v>
-      </c>
+      <c r="E54" s="1"/>
       <c r="F54" s="3">
         <f>F50-F52+F53</f>
         <v>0</v>
@@ -3201,17 +3258,18 @@
         <f>N50-N52+N53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:14">
+      <c r="O54" s="3">
+        <f>O50-O52+O53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:15">
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D56" s="1"/>
-      <c r="E56" s="4">
-        <f>Inputs!E$15</f>
-        <v>0</v>
-      </c>
+      <c r="E56" s="1"/>
       <c r="F56" s="4">
         <f>Inputs!F$15</f>
         <v>0</v>
@@ -3248,17 +3306,18 @@
         <f>Inputs!N$15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:14">
+      <c r="O56" s="4">
+        <f>Inputs!O$15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:15">
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D57" s="1"/>
-      <c r="E57" s="3">
-        <f>E54-E56</f>
-        <v>0</v>
-      </c>
+      <c r="E57" s="1"/>
       <c r="F57" s="3">
         <f>F54-F56</f>
         <v>0</v>
@@ -3293,6 +3352,10 @@
       </c>
       <c r="N57" s="3">
         <f>N54-N56</f>
+        <v>0</v>
+      </c>
+      <c r="O57" s="3">
+        <f>O54-O56</f>
         <v>0</v>
       </c>
     </row>
@@ -3303,22 +3366,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N13"/>
+  <dimension ref="B2:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:15">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="4">
-        <f>Inputs!E$17</f>
-        <v>0</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="4">
         <f>Inputs!F$17</f>
         <v>0</v>
@@ -3355,17 +3415,18 @@
         <f>Inputs!N$17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:14">
+      <c r="O2" s="4">
+        <f>Inputs!O$17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:15">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="3">
-        <f>'Balance Sheet'!E57</f>
-        <v>0</v>
-      </c>
+      <c r="E3" s="1"/>
       <c r="F3" s="3">
         <f>'Balance Sheet'!F57</f>
         <v>0</v>
@@ -3402,17 +3463,18 @@
         <f>'Balance Sheet'!N57</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="O3" s="3">
+        <f>'Balance Sheet'!O57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="4">
-        <f>Inputs!E$18</f>
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="4">
         <f>Inputs!F$18</f>
         <v>0</v>
@@ -3449,17 +3511,18 @@
         <f>Inputs!N$18</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:14">
+      <c r="O4" s="4">
+        <f>Inputs!O$18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="3">
-        <f>E2+E3+E4</f>
-        <v>0</v>
-      </c>
+      <c r="E5" s="1"/>
       <c r="F5" s="3">
         <f>F2+F3+F4</f>
         <v>0</v>
@@ -3496,17 +3559,18 @@
         <f>N2+N3+N4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:14">
+      <c r="O5" s="3">
+        <f>O2+O3+O4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:15">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1"/>
-      <c r="E7" s="4">
-        <f>Inputs!E$19</f>
-        <v>0</v>
-      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="4">
         <f>Inputs!F$19</f>
         <v>0</v>
@@ -3543,17 +3607,18 @@
         <f>Inputs!N$19</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
+      <c r="O7" s="4">
+        <f>Inputs!O$19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:15">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="1"/>
-      <c r="E8" s="4">
-        <f>Inputs!E$20</f>
-        <v>0</v>
-      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="4">
         <f>Inputs!F$20</f>
         <v>0</v>
@@ -3590,17 +3655,18 @@
         <f>Inputs!N$20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:14">
+      <c r="O8" s="4">
+        <f>Inputs!O$20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="1"/>
-      <c r="E9" s="3">
-        <f>E8*E7</f>
-        <v>0</v>
-      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="3">
         <f>F8*F7</f>
         <v>0</v>
@@ -3637,17 +3703,18 @@
         <f>N8*N7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:14">
+      <c r="O9" s="3">
+        <f>O8*O7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="4">
-        <f>Inputs!E$21</f>
-        <v>0</v>
-      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="4">
         <f>Inputs!F$21</f>
         <v>0</v>
@@ -3684,17 +3751,18 @@
         <f>Inputs!N$21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:14">
+      <c r="O11" s="4">
+        <f>Inputs!O$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="1"/>
-      <c r="E12" s="3">
-        <f>E7</f>
-        <v>0</v>
-      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="3">
         <f>F7</f>
         <v>0</v>
@@ -3731,17 +3799,18 @@
         <f>N7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
+      <c r="O12" s="3">
+        <f>O7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="3">
-        <f>E12*E11</f>
-        <v>0</v>
-      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="3">
         <f>F12*F11</f>
         <v>0</v>
@@ -3776,6 +3845,10 @@
       </c>
       <c r="N13" s="3">
         <f>N12*N11</f>
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <f>O12*O11</f>
         <v>0</v>
       </c>
     </row>
@@ -3786,22 +3859,19 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:N4"/>
+  <dimension ref="B2:O4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:15">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="1"/>
-      <c r="E2" s="3">
-        <f>Model!E9</f>
-        <v>0</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="3">
         <f>Model!F9</f>
         <v>0</v>
@@ -3838,17 +3908,18 @@
         <f>Model!N9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="O2" s="3">
+        <f>Model!O9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="E4" s="3">
-        <f>Model!E13</f>
-        <v>0</v>
-      </c>
+      <c r="E4" s="1"/>
       <c r="F4" s="3">
         <f>Model!F13</f>
         <v>0</v>
@@ -3883,6 +3954,10 @@
       </c>
       <c r="N4" s="3">
         <f>Model!N13</f>
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <f>Model!O13</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Make sure UOM's right is blank otherwise BB of corkscrew becomes error
</commit_message>
<xml_diff>
--- a/src/Tests/pickles/change_worksheet2_output.xlsx
+++ b/src/Tests/pickles/change_worksheet2_output.xlsx
@@ -506,22 +506,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O21"/>
+  <dimension ref="B2:P21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="2">
-        <v>0</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="2">
         <v>0</v>
       </c>
@@ -549,17 +547,18 @@
       <c r="O2" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
+      <c r="P2" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16">
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="2">
-        <v>0</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="2">
         <v>0</v>
       </c>
@@ -587,17 +586,18 @@
       <c r="O3" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="P3" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="2">
         <v>0</v>
       </c>
@@ -625,17 +625,18 @@
       <c r="O4" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="P4" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="2">
         <v>0</v>
       </c>
@@ -663,17 +664,18 @@
       <c r="O5" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:15">
+      <c r="P5" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="2">
         <v>0</v>
       </c>
@@ -701,17 +703,18 @@
       <c r="O6" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="P6" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="2">
         <v>0</v>
       </c>
@@ -739,17 +742,18 @@
       <c r="O7" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="P7" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="2">
         <v>0</v>
       </c>
@@ -777,17 +781,18 @@
       <c r="O8" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="P8" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="2">
         <v>0</v>
       </c>
@@ -815,17 +820,18 @@
       <c r="O9" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="P9" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="2">
-        <v>0</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="2">
         <v>0</v>
       </c>
@@ -853,17 +859,18 @@
       <c r="O10" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="P10" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="2">
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="2">
         <v>0</v>
       </c>
@@ -891,17 +898,18 @@
       <c r="O11" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="P11" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="2">
-        <v>0</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="2">
         <v>0</v>
       </c>
@@ -929,17 +937,18 @@
       <c r="O12" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="P12" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="B13" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="2">
-        <v>0</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="2">
         <v>0</v>
       </c>
@@ -967,17 +976,18 @@
       <c r="O13" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="P13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="2">
-        <v>0</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="2">
         <v>0</v>
       </c>
@@ -1005,17 +1015,18 @@
       <c r="O14" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="P14" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="2">
-        <v>0</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="2">
         <v>0</v>
       </c>
@@ -1043,17 +1054,18 @@
       <c r="O15" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="P15" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="2">
-        <v>0</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="2">
         <v>0</v>
       </c>
@@ -1081,17 +1093,18 @@
       <c r="O17" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:15">
+      <c r="P17" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="2">
-        <v>0</v>
-      </c>
+      <c r="F18" s="1"/>
       <c r="G18" s="2">
         <v>0</v>
       </c>
@@ -1119,17 +1132,18 @@
       <c r="O18" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="P18" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="2">
-        <v>0</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="2">
         <v>0</v>
       </c>
@@ -1157,17 +1171,18 @@
       <c r="O19" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:15">
+      <c r="P19" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="2">
-        <v>0</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="2">
         <v>0</v>
       </c>
@@ -1195,17 +1210,18 @@
       <c r="O20" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="P20" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="2">
-        <v>0</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="2">
         <v>0</v>
       </c>
@@ -1231,6 +1247,9 @@
         <v>0</v>
       </c>
       <c r="O21" s="2">
+        <v>0</v>
+      </c>
+      <c r="P21" s="2">
         <v>0</v>
       </c>
     </row>
@@ -1241,23 +1260,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O57"/>
+  <dimension ref="B2:P57"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:16">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="3">
-        <f>F30</f>
-        <v>0</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="3">
         <f>G30</f>
         <v>0</v>
@@ -1294,18 +1310,19 @@
         <f>O30</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
+      <c r="P2" s="3">
+        <f>P30</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="4">
-        <f>Inputs!F$2</f>
-        <v>0</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="4">
         <f>Inputs!G$2</f>
         <v>0</v>
@@ -1342,18 +1359,19 @@
         <f>Inputs!O$2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="P3" s="4">
+        <f>Inputs!P$2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="3">
-        <f>F2+F3</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="3">
         <f>G2+G3</f>
         <v>0</v>
@@ -1390,18 +1408,19 @@
         <f>O2+O3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="P4" s="3">
+        <f>P2+P3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4">
-        <f>Inputs!F$3</f>
-        <v>0</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="4">
         <f>Inputs!G$3</f>
         <v>0</v>
@@ -1438,18 +1457,19 @@
         <f>Inputs!O$3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:15">
+      <c r="P5" s="4">
+        <f>Inputs!P$3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16">
       <c r="B6" s="1"/>
       <c r="C6" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="3">
-        <f>F5+F4</f>
-        <v>0</v>
-      </c>
+      <c r="F6" s="1"/>
       <c r="G6" s="3">
         <f>G5+G4</f>
         <v>0</v>
@@ -1486,18 +1506,19 @@
         <f>O5+O4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="P6" s="3">
+        <f>P5+P4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4">
-        <f>Inputs!F$4</f>
-        <v>0</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="4">
         <f>Inputs!G$4</f>
         <v>0</v>
@@ -1534,18 +1555,19 @@
         <f>Inputs!O$4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="P8" s="4">
+        <f>Inputs!P$4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="3">
-        <f>F32</f>
-        <v>0</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="3">
         <f>G32</f>
         <v>0</v>
@@ -1582,18 +1604,19 @@
         <f>O32</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:15">
+      <c r="P9" s="3">
+        <f>P32</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:16">
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="3">
-        <f>F8+F9</f>
-        <v>0</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="3">
         <f>G8+G9</f>
         <v>0</v>
@@ -1630,18 +1653,19 @@
         <f>O8+O9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="P10" s="3">
+        <f>P8+P9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="4">
-        <f>Inputs!F$5</f>
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="4">
         <f>Inputs!G$5</f>
         <v>0</v>
@@ -1678,18 +1702,19 @@
         <f>Inputs!O$5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="P11" s="4">
+        <f>Inputs!P$5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="3">
-        <f>F11+F10</f>
-        <v>0</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="3">
         <f>G11+G10</f>
         <v>0</v>
@@ -1726,18 +1751,19 @@
         <f>O11+O10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:15">
+      <c r="P12" s="3">
+        <f>P11+P10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-      <c r="F14" s="4">
-        <f>Inputs!F$6</f>
-        <v>0</v>
-      </c>
+      <c r="F14" s="1"/>
       <c r="G14" s="4">
         <f>Inputs!G$6</f>
         <v>0</v>
@@ -1774,18 +1800,19 @@
         <f>Inputs!O$6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:15">
+      <c r="P14" s="4">
+        <f>Inputs!P$6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-      <c r="F15" s="3">
-        <f>Model!F5</f>
-        <v>0</v>
-      </c>
+      <c r="F15" s="1"/>
       <c r="G15" s="3">
         <f>Model!G5</f>
         <v>0</v>
@@ -1822,18 +1849,19 @@
         <f>Model!O5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:15">
+      <c r="P15" s="3">
+        <f>Model!P5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-      <c r="F16" s="4">
-        <f>Inputs!F$7</f>
-        <v>0</v>
-      </c>
+      <c r="F16" s="1"/>
       <c r="G16" s="4">
         <f>Inputs!G$7</f>
         <v>0</v>
@@ -1870,18 +1898,19 @@
         <f>Inputs!O$7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:15">
+      <c r="P16" s="4">
+        <f>Inputs!P$7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="3">
-        <f>F16+F15+F14</f>
-        <v>0</v>
-      </c>
+      <c r="F17" s="1"/>
       <c r="G17" s="3">
         <f>G16+G15+G14</f>
         <v>0</v>
@@ -1918,18 +1947,19 @@
         <f>O16+O15+O14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:15">
+      <c r="P17" s="3">
+        <f>P16+P15+P14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-      <c r="F19" s="3">
-        <f>F17</f>
-        <v>0</v>
-      </c>
+      <c r="F19" s="1"/>
       <c r="G19" s="3">
         <f>G17</f>
         <v>0</v>
@@ -1966,18 +1996,19 @@
         <f>O17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="2:15">
+      <c r="P19" s="3">
+        <f>P17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="3">
-        <f>F8</f>
-        <v>0</v>
-      </c>
+      <c r="F20" s="1"/>
       <c r="G20" s="3">
         <f>G8</f>
         <v>0</v>
@@ -2014,18 +2045,19 @@
         <f>O8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="2:15">
+      <c r="P20" s="3">
+        <f>P8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="3">
-        <f>F11</f>
-        <v>0</v>
-      </c>
+      <c r="F21" s="1"/>
       <c r="G21" s="3">
         <f>G11</f>
         <v>0</v>
@@ -2062,18 +2094,19 @@
         <f>O11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:15">
+      <c r="P21" s="3">
+        <f>P11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-      <c r="F23" s="3">
-        <f>F3</f>
-        <v>0</v>
-      </c>
+      <c r="F23" s="1"/>
       <c r="G23" s="3">
         <f>G3</f>
         <v>0</v>
@@ -2110,18 +2143,19 @@
         <f>O3</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="2:15">
+      <c r="P23" s="3">
+        <f>P3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-      <c r="F24" s="3">
-        <f>F5</f>
-        <v>0</v>
-      </c>
+      <c r="F24" s="1"/>
       <c r="G24" s="3">
         <f>G5</f>
         <v>0</v>
@@ -2158,18 +2192,19 @@
         <f>O5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:15">
+      <c r="P24" s="3">
+        <f>P5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
         <v>29</v>
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-      <c r="F25" s="3">
-        <f>F23+F24</f>
-        <v>0</v>
-      </c>
+      <c r="F25" s="1"/>
       <c r="G25" s="3">
         <f>G23+G24</f>
         <v>0</v>
@@ -2206,18 +2241,19 @@
         <f>O23+O24</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:15">
+      <c r="P25" s="3">
+        <f>P23+P24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-      <c r="F27" s="3">
-        <f>F19+F20+F21-F25</f>
-        <v>0</v>
-      </c>
+      <c r="F27" s="1"/>
       <c r="G27" s="3">
         <f>G19+G20+G21-G25</f>
         <v>0</v>
@@ -2254,18 +2290,19 @@
         <f>O19+O20+O21-O25</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:15">
+      <c r="P27" s="3">
+        <f>P19+P20+P21-P25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="3">
-        <f>max(0, F27)</f>
-        <v>0</v>
-      </c>
+      <c r="F29" s="1"/>
       <c r="G29" s="3">
         <f>max(0, G27)</f>
         <v>0</v>
@@ -2302,18 +2339,19 @@
         <f>max(0, O27)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="2:15">
+      <c r="P29" s="3">
+        <f>max(0, P27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
       <c r="B30" s="1"/>
       <c r="C30" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-      <c r="F30" s="3">
-        <f>F29</f>
-        <v>0</v>
-      </c>
+      <c r="F30" s="1"/>
       <c r="G30" s="3">
         <f>G29</f>
         <v>0</v>
@@ -2350,18 +2388,19 @@
         <f>O29</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="2:15">
+      <c r="P30" s="3">
+        <f>P29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
       <c r="B31" s="1"/>
       <c r="C31" s="1" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="3">
-        <f>min(F27, 0)</f>
-        <v>0</v>
-      </c>
+      <c r="F31" s="1"/>
       <c r="G31" s="3">
         <f>min(G27, 0)</f>
         <v>0</v>
@@ -2398,18 +2437,19 @@
         <f>min(O27, 0)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="2:15">
+      <c r="P31" s="3">
+        <f>min(P27, 0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
       <c r="B32" s="1"/>
       <c r="C32" s="1" t="s">
         <v>33</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="3">
-        <f>-1*F31</f>
-        <v>0</v>
-      </c>
+      <c r="F32" s="1"/>
       <c r="G32" s="3">
         <f>-1*G31</f>
         <v>0</v>
@@ -2446,18 +2486,19 @@
         <f>-1*O31</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:15">
+      <c r="P32" s="3">
+        <f>-1*P31</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
       <c r="B34" s="1"/>
       <c r="C34" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="3">
-        <f>F6</f>
-        <v>0</v>
-      </c>
+      <c r="F34" s="1"/>
       <c r="G34" s="3">
         <f>G6</f>
         <v>0</v>
@@ -2494,18 +2535,19 @@
         <f>O6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="2:15">
+      <c r="P34" s="3">
+        <f>P6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
       <c r="B35" s="1"/>
       <c r="C35" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="3">
-        <f>F12</f>
-        <v>0</v>
-      </c>
+      <c r="F35" s="1"/>
       <c r="G35" s="3">
         <f>G12</f>
         <v>0</v>
@@ -2542,18 +2584,19 @@
         <f>O12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="2:15">
+      <c r="P35" s="3">
+        <f>P12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
       <c r="B36" s="1"/>
       <c r="C36" s="1" t="s">
         <v>26</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-      <c r="F36" s="3">
-        <f>F17</f>
-        <v>0</v>
-      </c>
+      <c r="F36" s="1"/>
       <c r="G36" s="3">
         <f>G17</f>
         <v>0</v>
@@ -2590,18 +2633,19 @@
         <f>O17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="37" spans="2:15">
+      <c r="P36" s="3">
+        <f>P17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
       <c r="B37" s="1"/>
       <c r="C37" s="1" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="3">
-        <f>F34-(F35+F36)</f>
-        <v>0</v>
-      </c>
+      <c r="F37" s="1"/>
       <c r="G37" s="3">
         <f>G34-(G35+G36)</f>
         <v>0</v>
@@ -2638,18 +2682,19 @@
         <f>O34-(O35+O36)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="2:15">
+      <c r="P37" s="3">
+        <f>P34-(P35+P36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
       <c r="B39" s="1"/>
       <c r="C39" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="3">
-        <f>'Core Accounts'!F2</f>
-        <v>0</v>
-      </c>
+      <c r="F39" s="1"/>
       <c r="G39" s="3">
         <f>'Core Accounts'!G2</f>
         <v>0</v>
@@ -2686,18 +2731,19 @@
         <f>'Core Accounts'!O2</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="2:15">
+      <c r="P39" s="3">
+        <f>'Core Accounts'!P2</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16">
       <c r="B40" s="1"/>
       <c r="C40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="3">
-        <f>'Core Accounts'!F4</f>
-        <v>0</v>
-      </c>
+      <c r="F40" s="1"/>
       <c r="G40" s="3">
         <f>'Core Accounts'!G4</f>
         <v>0</v>
@@ -2734,18 +2780,19 @@
         <f>'Core Accounts'!O4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="41" spans="2:15">
+      <c r="P40" s="3">
+        <f>'Core Accounts'!P4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16">
       <c r="B41" s="1"/>
       <c r="C41" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="3">
-        <f>F39-F40</f>
-        <v>0</v>
-      </c>
+      <c r="F41" s="1"/>
       <c r="G41" s="3">
         <f>G39-G40</f>
         <v>0</v>
@@ -2782,18 +2829,19 @@
         <f>O39-O40</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="43" spans="2:15">
+      <c r="P41" s="3">
+        <f>P39-P40</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
       <c r="B43" s="1"/>
       <c r="C43" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="4">
-        <f>Inputs!F$8</f>
-        <v>0</v>
-      </c>
+      <c r="F43" s="1"/>
       <c r="G43" s="4">
         <f>Inputs!G$8</f>
         <v>0</v>
@@ -2830,18 +2878,19 @@
         <f>Inputs!O$8</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="2:15">
+      <c r="P43" s="4">
+        <f>Inputs!P$8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16">
       <c r="B44" s="1"/>
       <c r="C44" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="4">
-        <f>Inputs!F$9</f>
-        <v>0</v>
-      </c>
+      <c r="F44" s="1"/>
       <c r="G44" s="4">
         <f>Inputs!G$9</f>
         <v>0</v>
@@ -2878,18 +2927,19 @@
         <f>Inputs!O$9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="45" spans="2:15">
+      <c r="P44" s="4">
+        <f>Inputs!P$9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16">
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="4">
-        <f>Inputs!F$10</f>
-        <v>0</v>
-      </c>
+      <c r="F45" s="1"/>
       <c r="G45" s="4">
         <f>Inputs!G$10</f>
         <v>0</v>
@@ -2926,18 +2976,19 @@
         <f>Inputs!O$10</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="2:15">
+      <c r="P45" s="4">
+        <f>Inputs!P$10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
       <c r="B46" s="1"/>
       <c r="C46" s="1" t="s">
         <v>38</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="3">
-        <f>F41-(F43+F44)+F45</f>
-        <v>0</v>
-      </c>
+      <c r="F46" s="1"/>
       <c r="G46" s="3">
         <f>G41-(G43+G44)+G45</f>
         <v>0</v>
@@ -2974,18 +3025,19 @@
         <f>O41-(O43+O44)+O45</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="2:15">
+      <c r="P46" s="3">
+        <f>P41-(P43+P44)+P45</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16">
       <c r="B48" s="1"/>
       <c r="C48" s="1" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="4">
-        <f>Inputs!F$11</f>
-        <v>0</v>
-      </c>
+      <c r="F48" s="1"/>
       <c r="G48" s="4">
         <f>Inputs!G$11</f>
         <v>0</v>
@@ -3022,18 +3074,19 @@
         <f>Inputs!O$11</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="49" spans="2:15">
+      <c r="P48" s="4">
+        <f>Inputs!P$11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="2:16">
       <c r="B49" s="1"/>
       <c r="C49" s="1" t="s">
         <v>10</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="4">
-        <f>Inputs!F$12</f>
-        <v>0</v>
-      </c>
+      <c r="F49" s="1"/>
       <c r="G49" s="4">
         <f>Inputs!G$12</f>
         <v>0</v>
@@ -3070,18 +3123,19 @@
         <f>Inputs!O$12</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="2:15">
+      <c r="P49" s="4">
+        <f>Inputs!P$12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:16">
       <c r="B50" s="1"/>
       <c r="C50" s="1" t="s">
         <v>39</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="3">
-        <f>F46-(F48+F49)</f>
-        <v>0</v>
-      </c>
+      <c r="F50" s="1"/>
       <c r="G50" s="3">
         <f>G46-(G48+G49)</f>
         <v>0</v>
@@ -3118,18 +3172,19 @@
         <f>O46-(O48+O49)</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="52" spans="2:15">
+      <c r="P50" s="3">
+        <f>P46-(P48+P49)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:16">
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="4">
-        <f>Inputs!F$13</f>
-        <v>0</v>
-      </c>
+      <c r="F52" s="1"/>
       <c r="G52" s="4">
         <f>Inputs!G$13</f>
         <v>0</v>
@@ -3166,18 +3221,19 @@
         <f>Inputs!O$13</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="53" spans="2:15">
+      <c r="P52" s="4">
+        <f>Inputs!P$13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:16">
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="4">
-        <f>Inputs!F$14</f>
-        <v>0</v>
-      </c>
+      <c r="F53" s="1"/>
       <c r="G53" s="4">
         <f>Inputs!G$14</f>
         <v>0</v>
@@ -3214,18 +3270,19 @@
         <f>Inputs!O$14</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="54" spans="2:15">
+      <c r="P53" s="4">
+        <f>Inputs!P$14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:16">
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>40</v>
       </c>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="3">
-        <f>F50-F52+F53</f>
-        <v>0</v>
-      </c>
+      <c r="F54" s="1"/>
       <c r="G54" s="3">
         <f>G50-G52+G53</f>
         <v>0</v>
@@ -3262,18 +3319,19 @@
         <f>O50-O52+O53</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="2:15">
+      <c r="P54" s="3">
+        <f>P50-P52+P53</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="2:16">
       <c r="B56" s="1"/>
       <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
-      <c r="F56" s="4">
-        <f>Inputs!F$15</f>
-        <v>0</v>
-      </c>
+      <c r="F56" s="1"/>
       <c r="G56" s="4">
         <f>Inputs!G$15</f>
         <v>0</v>
@@ -3310,18 +3368,19 @@
         <f>Inputs!O$15</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="2:15">
+      <c r="P56" s="4">
+        <f>Inputs!P$15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="2:16">
       <c r="B57" s="1"/>
       <c r="C57" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="3">
-        <f>F54-F56</f>
-        <v>0</v>
-      </c>
+      <c r="F57" s="1"/>
       <c r="G57" s="3">
         <f>G54-G56</f>
         <v>0</v>
@@ -3356,6 +3415,10 @@
       </c>
       <c r="O57" s="3">
         <f>O54-O56</f>
+        <v>0</v>
+      </c>
+      <c r="P57" s="3">
+        <f>P54-P56</f>
         <v>0</v>
       </c>
     </row>
@@ -3366,23 +3429,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O13"/>
+  <dimension ref="B2:P13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:16">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="4">
-        <f>Inputs!F$17</f>
-        <v>0</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="4">
         <f>Inputs!G$17</f>
         <v>0</v>
@@ -3419,18 +3479,19 @@
         <f>Inputs!O$17</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="2:15">
+      <c r="P2" s="4">
+        <f>Inputs!P$17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="2:16">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="3">
-        <f>'Balance Sheet'!F57</f>
-        <v>0</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="G3" s="3">
         <f>'Balance Sheet'!G57</f>
         <v>0</v>
@@ -3467,18 +3528,19 @@
         <f>'Balance Sheet'!O57</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="P3" s="3">
+        <f>'Balance Sheet'!P57</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4">
-        <f>Inputs!F$18</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="4">
         <f>Inputs!G$18</f>
         <v>0</v>
@@ -3515,18 +3577,19 @@
         <f>Inputs!O$18</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="2:15">
+      <c r="P4" s="4">
+        <f>Inputs!P$18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16">
       <c r="B5" s="1"/>
       <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="3">
-        <f>F2+F3+F4</f>
-        <v>0</v>
-      </c>
+      <c r="F5" s="1"/>
       <c r="G5" s="3">
         <f>G2+G3+G4</f>
         <v>0</v>
@@ -3563,18 +3626,19 @@
         <f>O2+O3+O4</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:15">
+      <c r="P5" s="3">
+        <f>P2+P3+P4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16">
       <c r="B7" s="1"/>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="4">
-        <f>Inputs!F$19</f>
-        <v>0</v>
-      </c>
+      <c r="F7" s="1"/>
       <c r="G7" s="4">
         <f>Inputs!G$19</f>
         <v>0</v>
@@ -3611,18 +3675,19 @@
         <f>Inputs!O$19</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:15">
+      <c r="P7" s="4">
+        <f>Inputs!P$19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16">
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="4">
-        <f>Inputs!F$20</f>
-        <v>0</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="4">
         <f>Inputs!G$20</f>
         <v>0</v>
@@ -3659,18 +3724,19 @@
         <f>Inputs!O$20</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:15">
+      <c r="P8" s="4">
+        <f>Inputs!P$20</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16">
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="3">
-        <f>F8*F7</f>
-        <v>0</v>
-      </c>
+      <c r="F9" s="1"/>
       <c r="G9" s="3">
         <f>G8*G7</f>
         <v>0</v>
@@ -3707,18 +3773,19 @@
         <f>O8*O7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:15">
+      <c r="P9" s="3">
+        <f>P8*P7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:16">
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="4">
-        <f>Inputs!F$21</f>
-        <v>0</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="4">
         <f>Inputs!G$21</f>
         <v>0</v>
@@ -3755,18 +3822,19 @@
         <f>Inputs!O$21</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="2:15">
+      <c r="P11" s="4">
+        <f>Inputs!P$21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:16">
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="3">
-        <f>F7</f>
-        <v>0</v>
-      </c>
+      <c r="F12" s="1"/>
       <c r="G12" s="3">
         <f>G7</f>
         <v>0</v>
@@ -3803,18 +3871,19 @@
         <f>O7</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:15">
+      <c r="P12" s="3">
+        <f>P7</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:16">
       <c r="B13" s="1"/>
       <c r="C13" s="1" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-      <c r="F13" s="3">
-        <f>F12*F11</f>
-        <v>0</v>
-      </c>
+      <c r="F13" s="1"/>
       <c r="G13" s="3">
         <f>G12*G11</f>
         <v>0</v>
@@ -3849,6 +3918,10 @@
       </c>
       <c r="O13" s="3">
         <f>O12*O11</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <f>P12*P11</f>
         <v>0</v>
       </c>
     </row>
@@ -3859,23 +3932,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:O4"/>
+  <dimension ref="B2:P4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="2" spans="2:15">
+    <row r="2" spans="2:16">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>43</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
-      <c r="F2" s="3">
-        <f>Model!F9</f>
-        <v>0</v>
-      </c>
+      <c r="F2" s="1"/>
       <c r="G2" s="3">
         <f>Model!G9</f>
         <v>0</v>
@@ -3912,18 +3982,19 @@
         <f>Model!O9</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:15">
+      <c r="P2" s="3">
+        <f>Model!P9</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:16">
       <c r="B4" s="1"/>
       <c r="C4" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="3">
-        <f>Model!F13</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="1"/>
       <c r="G4" s="3">
         <f>Model!G13</f>
         <v>0</v>
@@ -3958,6 +4029,10 @@
       </c>
       <c r="O4" s="3">
         <f>Model!O13</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="3">
+        <f>Model!P13</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Extract copy to clipboard to Utilities
</commit_message>
<xml_diff>
--- a/src/Tests/pickles/change_worksheet2_output.xlsx
+++ b/src/Tests/pickles/change_worksheet2_output.xlsx
@@ -511,6 +511,25 @@
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1" t="s">
@@ -1265,6 +1284,25 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1"/>
@@ -3434,6 +3472,25 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1"/>
@@ -3937,6 +3994,25 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="2.7109375" customWidth="1"/>
+    <col min="2" max="2" width="2.7109375" customWidth="1"/>
+    <col min="3" max="3" width="2.7109375" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" customWidth="1"/>
+    <col min="6" max="6" width="2.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="15.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="15.7109375" customWidth="1"/>
+    <col min="11" max="11" width="15.7109375" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="15" max="15" width="15.7109375" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" customWidth="1"/>
+    <col min="17" max="16384" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:16">
       <c r="B2" s="1"/>

</xml_diff>